<commit_message>
Update of the documentation with fitting and single crystal stuff described
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,11 +4,11 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="9660" windowHeight="8050"/>
+    <workbookView activeTab="0" windowWidth="20000" windowHeight="8050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Development" sheetId="1" r:id="rId1"/>
+    <sheet name="SpeedUp" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+  <si>
+    <t>Total</t>
+  </si>
   <si>
     <t>Linux</t>
   </si>
@@ -40,6 +43,12 @@
   </si>
   <si>
     <t>Windows</t>
+  </si>
+  <si>
+    <t>Processors</t>
+  </si>
+  <si>
+    <t>system</t>
   </si>
 </sst>
 </file>
@@ -91,12 +100,20 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
@@ -109,25 +126,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="10.999338942307693" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" style="0" width="16.28473557692308" customWidth="1"/>
+    <col min="1" max="1" style="0" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="0" width="16.28515625" customWidth="1"/>
     <col min="3" max="5" style="0" width="9.142307692307693"/>
-    <col min="6" max="6" style="0" width="9.285156250000002" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" style="0" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Timings for running </t>
+          <t>Timings for running</t>
         </is>
       </c>
     </row>
@@ -164,10 +181,8 @@
           <t>System%</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
+      <c r="F4" t="s">
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -207,10 +222,10 @@
         <v>296.36000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -235,10 +250,10 @@
         <v>294.24000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -263,10 +278,10 @@
         <v>251.06</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -279,7 +294,7 @@
         <v>44498</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>589.29999999999995</v>
@@ -294,10 +309,10 @@
         <v>232.59</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -310,7 +325,7 @@
         <v>44498</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>469.01999999999998</v>
@@ -325,10 +340,10 @@
         <v>107.65000000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -341,7 +356,7 @@
         <v>44498</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>599.09000000000003</v>
@@ -356,10 +371,10 @@
         <v>346.07999999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -372,7 +387,7 @@
         <v>44498</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -384,10 +399,10 @@
         <v>1419.2529999999999</v>
       </c>
       <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
         <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -395,7 +410,7 @@
         <v>44498</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -407,14 +422,128 @@
         <v>1104.95</v>
       </c>
       <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" t="s">
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
+        <v>44504</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
+      <c r="C13">
+        <v>469.5</v>
+      </c>
+      <c r="D13">
+        <v>20.219999999999999</v>
+      </c>
+      <c r="E13">
+        <v>444</v>
+      </c>
+      <c r="F13">
+        <v>110.23999999999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2">
+        <v>44505</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1612</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Running in a command shell</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2">
+        <v>44505</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1214</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13.5">
+      <c r="A16" s="1">
+        <v>44510</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>465.02999999999997</v>
+      </c>
+      <c r="D16">
+        <v>19.629999999999999</v>
+      </c>
+      <c r="E16">
+        <v>451</v>
+      </c>
+      <c r="F16">
+        <v>107.29000000000001</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Getting ready to release</t>
         </is>
       </c>
     </row>
@@ -435,17 +564,707 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C1" sqref="C1:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="2" style="0" width="9.142307692307693"/>
+    <col min="3" max="3" style="0" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" style="0" width="9.142307692307693"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Speedup</t>
+        </is>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>409.09000000000003</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>510.43s</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>46.28s</t>
+        </is>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.3600000000000001</v>
+      </c>
+      <c r="J2">
+        <f>K2*60+L2</f>
+        <v>409.09000000000003</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>49.090000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>220.42000000000002</v>
+      </c>
+      <c r="C3">
+        <f>$B$2/B3</f>
+        <v>1.855956809726885</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>416.67s</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>8.18s</t>
+        </is>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.9199999999999999</v>
+      </c>
+      <c r="J3">
+        <f>K3*60+L3</f>
+        <v>220.42000000000002</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>40.420000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>169.19999999999999</v>
+      </c>
+      <c r="C4">
+        <f>$B$2/B4</f>
+        <v>2.4177895981087474</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>426.44s</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10.06s</t>
+        </is>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.5699999999999998</v>
+      </c>
+      <c r="J4">
+        <f>K4*60+L4</f>
+        <v>169.19999999999999</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>49.200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>143.93000000000001</v>
+      </c>
+      <c r="C5">
+        <f>$B$2/B5</f>
+        <v>2.8422844438268604</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>437.15s</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>11.59s</t>
+        </is>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.1099999999999999</v>
+      </c>
+      <c r="J5">
+        <f>K5*60+L5</f>
+        <v>143.93000000000001</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>23.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>127.84</v>
+      </c>
+      <c r="C6">
+        <f>$B$2/B6</f>
+        <v>3.2000156445556946</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>440.41s</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>13.09s</t>
+        </is>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.54</v>
+      </c>
+      <c r="J6">
+        <f>K6*60+L6</f>
+        <v>127.84</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>7.8399999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>117.64</v>
+      </c>
+      <c r="C7">
+        <f>$B$2/B7</f>
+        <v>3.4774736484189055</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>444.30s</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>14.94s</t>
+        </is>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.8999999999999999</v>
+      </c>
+      <c r="J7">
+        <f>K7*60+L7</f>
+        <v>117.64</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>57.640000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>112.44</v>
+      </c>
+      <c r="C8">
+        <f>$B$2/B8</f>
+        <v>3.6382959800782642</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>455.16s</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>17.51s</t>
+        </is>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4.2000000000000002</v>
+      </c>
+      <c r="J8">
+        <f>K8*60+L8</f>
+        <v>112.44</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>52.439999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>108.89</v>
+      </c>
+      <c r="C9">
+        <f>$B$2/B9</f>
+        <v>3.7569106437689412</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>470.99s</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20.22s</t>
+        </is>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4.5099999999999998</v>
+      </c>
+      <c r="J9">
+        <f>K9*60+L9</f>
+        <v>108.89</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>48.890000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>109.97</v>
+      </c>
+      <c r="C10">
+        <f>$B$2/B10</f>
+        <v>3.72001454942257</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>516.01s</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>22.69s</t>
+        </is>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="J10">
+        <f>K10*60+L10</f>
+        <v>109.97</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>49.969999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>111.69</v>
+      </c>
+      <c r="C11">
+        <f>$B$2/B11</f>
+        <v>3.6627271913331545</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>565.30s</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>24.69s</t>
+        </is>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5.2800000000000002</v>
+      </c>
+      <c r="J11">
+        <f>K11*60+L11</f>
+        <v>111.69</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>51.689999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>111.11</v>
+      </c>
+      <c r="C12">
+        <f>$B$2/B12</f>
+        <v>3.681846818468185</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>608.05s</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>27.83s</t>
+        </is>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="3">
+        <v>5.7199999999999998</v>
+      </c>
+      <c r="J12">
+        <f>K12*60+L12</f>
+        <v>111.11</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>51.109999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>111.86</v>
+      </c>
+      <c r="C13">
+        <f>$B$2/B13</f>
+        <v>3.6571607366350798</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>657.91s</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>31.55s</t>
+        </is>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="3">
+        <v>6.1600000000000001</v>
+      </c>
+      <c r="J13">
+        <f>K13*60+L13</f>
+        <v>111.86</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>51.859999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>113.03</v>
+      </c>
+      <c r="C14">
+        <f>$B$2/B14</f>
+        <v>3.6193046093957357</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>699.08s</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>35.96s</t>
+        </is>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J14">
+        <f>K14*60+L14</f>
+        <v>113.03</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>53.030000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>113.22</v>
+      </c>
+      <c r="C15">
+        <f>$B$2/B15</f>
+        <v>3.6132308779367608</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>742.17s</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>40.00s</t>
+        </is>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="3">
+        <v>6.9000000000000004</v>
+      </c>
+      <c r="J15">
+        <f>K15*60+L15</f>
+        <v>113.22</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>53.219999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>114.89</v>
+      </c>
+      <c r="C16">
+        <f>$B$2/B16</f>
+        <v>3.5607102445817742</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>788.81s</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>45.20s</t>
+        </is>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="J16">
+        <f>K16*60+L16</f>
+        <v>114.89</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>54.890000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>115.74000000000001</v>
+      </c>
+      <c r="C17">
+        <f>$B$2/B17</f>
+        <v>3.5345602211854157</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>821.18s</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>52.66s</t>
+        </is>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="3">
+        <v>7.54</v>
+      </c>
+      <c r="J17">
+        <f>K17*60+L17</f>
+        <v>115.74000000000001</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>55.740000000000002</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
@@ -468,9 +1287,10 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="0" width="9.142307692307693"/>
+    <col min="2" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Attempted to optimise the chunksize
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>Total</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Windows</t>
+  </si>
+  <si>
+    <t>Chunksize = 100</t>
+  </si>
+  <si>
+    <t>Chunksize = 20</t>
+  </si>
+  <si>
+    <t>Chunksize = 10</t>
   </si>
   <si>
     <t>Processors</t>
@@ -126,10 +135,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0" tabSelected="1">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -544,6 +553,186 @@
       <c r="L16" t="inlineStr">
         <is>
           <t>Getting ready to release</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5">
+      <c r="A17" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>464.89999999999998</v>
+      </c>
+      <c r="D17">
+        <v>15.609999999999999</v>
+      </c>
+      <c r="E17">
+        <v>434</v>
+      </c>
+      <c r="F17">
+        <v>110.62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Switch from imap to map</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.5">
+      <c r="A18" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>500.31</v>
+      </c>
+      <c r="D18">
+        <v>16.879999999999999</v>
+      </c>
+      <c r="E18">
+        <v>445</v>
+      </c>
+      <c r="F18">
+        <v>115.90000000000001</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Switching back to imap</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5">
+      <c r="A19" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>450.25999999999999</v>
+      </c>
+      <c r="D19">
+        <v>15.960000000000001</v>
+      </c>
+      <c r="E19">
+        <v>401</v>
+      </c>
+      <c r="F19">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.5">
+      <c r="A20" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>485.97000000000003</v>
+      </c>
+      <c r="D20">
+        <v>16.629999999999999</v>
+      </c>
+      <c r="E20">
+        <v>450</v>
+      </c>
+      <c r="F20">
+        <v>111.48999999999999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5">
+      <c r="A21" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>490.81999999999999</v>
+      </c>
+      <c r="D21">
+        <v>18.460000000000001</v>
+      </c>
+      <c r="E21">
+        <v>450</v>
+      </c>
+      <c r="F21">
+        <v>113.12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5">
+      <c r="A22" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>532.49000000000001</v>
+      </c>
+      <c r="D22">
+        <v>19.66</v>
+      </c>
+      <c r="E22">
+        <v>447</v>
+      </c>
+      <c r="F22">
+        <v>123.36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Chunksize = 5</t>
         </is>
       </c>
     </row>
@@ -579,7 +768,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -590,7 +779,7 @@
         </is>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F1" t="inlineStr">
         <is>
@@ -598,7 +787,7 @@
         </is>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" t="inlineStr">
         <is>
@@ -633,7 +822,7 @@
         </is>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3">
         <v>1.3600000000000001</v>
@@ -674,7 +863,7 @@
         </is>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3">
         <v>1.9199999999999999</v>
@@ -715,7 +904,7 @@
         </is>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3">
         <v>2.5699999999999998</v>
@@ -756,7 +945,7 @@
         </is>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I5" s="3">
         <v>3.1099999999999999</v>
@@ -797,7 +986,7 @@
         </is>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3">
         <v>3.54</v>
@@ -838,7 +1027,7 @@
         </is>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I7" s="3">
         <v>3.8999999999999999</v>
@@ -879,7 +1068,7 @@
         </is>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3">
         <v>4.2000000000000002</v>
@@ -920,7 +1109,7 @@
         </is>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3">
         <v>4.5099999999999998</v>
@@ -961,7 +1150,7 @@
         </is>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I10" s="3">
         <v>4.8899999999999997</v>
@@ -1002,7 +1191,7 @@
         </is>
       </c>
       <c r="H11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I11" s="3">
         <v>5.2800000000000002</v>
@@ -1043,7 +1232,7 @@
         </is>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3">
         <v>5.7199999999999998</v>
@@ -1084,7 +1273,7 @@
         </is>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I13" s="3">
         <v>6.1600000000000001</v>
@@ -1125,7 +1314,7 @@
         </is>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I14" s="3">
         <v>6.5</v>
@@ -1166,7 +1355,7 @@
         </is>
       </c>
       <c r="H15" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I15" s="3">
         <v>6.9000000000000004</v>
@@ -1207,7 +1396,7 @@
         </is>
       </c>
       <c r="H16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I16" s="3">
         <v>7.25</v>
@@ -1248,7 +1437,7 @@
         </is>
       </c>
       <c r="H17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I17" s="3">
         <v>7.54</v>
@@ -1289,8 +1478,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Added Laptop linux results
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="20000" windowHeight="8050"/>
+    <workbookView activeTab="0" windowWidth="19200" windowHeight="8050"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>Total</t>
   </si>
@@ -42,16 +42,10 @@
     <t>Intel skylake (core m7) Intel Core(TM)i7-6500U@2.50GHz</t>
   </si>
   <si>
-    <t>Windows</t>
+    <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
   </si>
   <si>
-    <t>Chunksize = 100</t>
-  </si>
-  <si>
-    <t>Chunksize = 20</t>
-  </si>
-  <si>
-    <t>Chunksize = 10</t>
+    <t>Windows</t>
   </si>
   <si>
     <t>Processors</t>
@@ -135,10 +129,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0" tabSelected="1">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -385,10 +379,8 @@
       <c r="H10" t="s">
         <v>4</v>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
-        </is>
+      <c r="L10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -408,7 +400,7 @@
         <v>1419.2529999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -431,7 +423,7 @@
         <v>1104.95</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
@@ -488,7 +480,7 @@
         <v>1612</v>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" t="s">
         <v>4</v>
@@ -519,7 +511,7 @@
         <v>1214</v>
       </c>
       <c r="G15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
@@ -643,8 +635,10 @@
       <c r="H19" t="s">
         <v>2</v>
       </c>
-      <c r="L19" t="s">
-        <v>6</v>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Chunksize = 100</t>
+        </is>
       </c>
     </row>
     <row r="20" spans="1:12" ht="13.5">
@@ -672,8 +666,10 @@
       <c r="H20" t="s">
         <v>2</v>
       </c>
-      <c r="L20" t="s">
-        <v>7</v>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Chunksize = 20</t>
+        </is>
       </c>
     </row>
     <row r="21" spans="1:12" ht="13.5">
@@ -701,8 +697,10 @@
       <c r="H21" t="s">
         <v>2</v>
       </c>
-      <c r="L21" t="s">
-        <v>8</v>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Chunksize = 10</t>
+        </is>
       </c>
     </row>
     <row r="22" spans="1:12" ht="13.5">
@@ -733,6 +731,37 @@
       <c r="L22" t="inlineStr">
         <is>
           <t>Chunksize = 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.5">
+      <c r="A23" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>619.51999999999998</v>
+      </c>
+      <c r="D23">
+        <v>11.359999999999999</v>
+      </c>
+      <c r="E23">
+        <v>177</v>
+      </c>
+      <c r="F23">
+        <v>355.06999999999999</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Using new chunk sizes</t>
         </is>
       </c>
     </row>
@@ -768,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -779,7 +808,7 @@
         </is>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" t="inlineStr">
         <is>
@@ -787,7 +816,7 @@
         </is>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I1" t="inlineStr">
         <is>
@@ -822,7 +851,7 @@
         </is>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I2" s="3">
         <v>1.3600000000000001</v>
@@ -863,7 +892,7 @@
         </is>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3">
         <v>1.9199999999999999</v>
@@ -904,7 +933,7 @@
         </is>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4" s="3">
         <v>2.5699999999999998</v>
@@ -945,7 +974,7 @@
         </is>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" s="3">
         <v>3.1099999999999999</v>
@@ -986,7 +1015,7 @@
         </is>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I6" s="3">
         <v>3.54</v>
@@ -1027,7 +1056,7 @@
         </is>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I7" s="3">
         <v>3.8999999999999999</v>
@@ -1068,7 +1097,7 @@
         </is>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I8" s="3">
         <v>4.2000000000000002</v>
@@ -1109,7 +1138,7 @@
         </is>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9" s="3">
         <v>4.5099999999999998</v>
@@ -1150,7 +1179,7 @@
         </is>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I10" s="3">
         <v>4.8899999999999997</v>
@@ -1191,7 +1220,7 @@
         </is>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I11" s="3">
         <v>5.2800000000000002</v>
@@ -1232,7 +1261,7 @@
         </is>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I12" s="3">
         <v>5.7199999999999998</v>
@@ -1273,7 +1302,7 @@
         </is>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I13" s="3">
         <v>6.1600000000000001</v>
@@ -1314,7 +1343,7 @@
         </is>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I14" s="3">
         <v>6.5</v>
@@ -1355,7 +1384,7 @@
         </is>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I15" s="3">
         <v>6.9000000000000004</v>
@@ -1396,7 +1425,7 @@
         </is>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I16" s="3">
         <v>7.25</v>
@@ -1437,7 +1466,7 @@
         </is>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I17" s="3">
         <v>7.54</v>

</xml_diff>

<commit_message>
A few more tweaks to the documentation
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="20000" windowHeight="8050"/>
+    <workbookView activeTab="0" windowWidth="12800" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
   <si>
     <t>Total</t>
   </si>
@@ -45,13 +45,7 @@
     <t>Intel skylake (core m7) Intel Core(TM)i7-6500U@2.50GHz</t>
   </si>
   <si>
-    <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
-  </si>
-  <si>
-    <t>Processors</t>
-  </si>
-  <si>
-    <t>system</t>
+    <t>Default settings, but NUM_THREAD, OMP_NUM_THREAD set to 1</t>
   </si>
 </sst>
 </file>
@@ -125,10 +119,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -985,8 +979,10 @@
       <c r="H32" t="s">
         <v>5</v>
       </c>
-      <c r="L32" t="s">
-        <v>6</v>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
+        </is>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5">
@@ -1006,10 +1002,28 @@
       <c r="H33" t="s">
         <v>5</v>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Default settings, but NUM_THREAD, OMP_NUM_THREAD set to 1</t>
-        </is>
+      <c r="L33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5">
+      <c r="A34" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>358.08999999999997</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1029,10 +1043,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1042,9 +1056,11 @@
     <col min="4" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
-        <v>7</v>
+    <row r="1" spans="1:9">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Processors</t>
+        </is>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1054,680 +1070,137 @@
           <t>Speedup</t>
         </is>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>user</t>
-        </is>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>cpu</t>
-        </is>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:9" ht="13.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>409.09000000000003</v>
+        <f>6*60+23.5</f>
+        <v>383.5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>510.43s</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>46.28s</t>
-        </is>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1.3600000000000001</v>
-      </c>
-      <c r="J2">
-        <f>K2*60+L2</f>
-        <v>409.09000000000003</v>
-      </c>
-      <c r="K2">
-        <v>6</v>
-      </c>
-      <c r="L2">
-        <v>49.090000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>220.42000000000002</v>
+        <f>3*60+5.2999999999999998</f>
+        <v>185.30000000000001</v>
       </c>
       <c r="C3">
         <f>$B$2/B3</f>
-        <v>1.855956809726885</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>416.67s</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>8.18s</t>
-        </is>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1.9199999999999999</v>
-      </c>
-      <c r="J3">
-        <f>K3*60+L3</f>
-        <v>220.42000000000002</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>40.420000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>2.0696168375607122</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>169.19999999999999</v>
+        <f>2*60+22.300000000000001</f>
+        <v>142.30000000000001</v>
       </c>
       <c r="C4">
         <f>$B$2/B4</f>
-        <v>2.4177895981087474</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>426.44s</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>10.06s</t>
-        </is>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.5699999999999998</v>
-      </c>
-      <c r="J4">
-        <f>K4*60+L4</f>
-        <v>169.19999999999999</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>49.200000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>2.6950105411103302</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>143.93000000000001</v>
+        <f>124.16</f>
+        <v>124.16</v>
       </c>
       <c r="C5">
         <f>$B$2/B5</f>
-        <v>2.8422844438268604</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>437.15s</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>11.59s</t>
-        </is>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3.1099999999999999</v>
-      </c>
-      <c r="J5">
-        <f>K5*60+L5</f>
-        <v>143.93000000000001</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>23.93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>3.0887564432989691</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>127.84</v>
+        <v>110.08</v>
       </c>
       <c r="C6">
         <f>$B$2/B6</f>
-        <v>3.2000156445556946</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>440.41s</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>13.09s</t>
-        </is>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3.54</v>
-      </c>
-      <c r="J6">
-        <f>K6*60+L6</f>
-        <v>127.84</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>7.8399999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>3.4838299418604652</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>117.64</v>
+        <v>103.05</v>
       </c>
       <c r="C7">
         <f>$B$2/B7</f>
-        <v>3.4774736484189055</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>444.30s</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>14.94s</t>
-        </is>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3.8999999999999999</v>
-      </c>
-      <c r="J7">
-        <f>K7*60+L7</f>
-        <v>117.64</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>57.640000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>3.7214944201843765</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>112.44</v>
+        <v>96.069999999999993</v>
       </c>
       <c r="C8">
         <f>$B$2/B8</f>
-        <v>3.6382959800782642</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>455.16s</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>17.51s</t>
-        </is>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="2">
-        <v>4.2000000000000002</v>
-      </c>
-      <c r="J8">
-        <f>K8*60+L8</f>
-        <v>112.44</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>52.439999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>3.9918809201623819</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>108.89</v>
+        <v>92.640000000000001</v>
       </c>
       <c r="C9">
         <f>$B$2/B9</f>
-        <v>3.7569106437689412</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>470.99s</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>20.22s</t>
-        </is>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4.5099999999999998</v>
-      </c>
-      <c r="J9">
-        <f>K9*60+L9</f>
-        <v>108.89</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>48.890000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>109.97</v>
-      </c>
-      <c r="C10">
-        <f>$B$2/B10</f>
-        <v>3.72001454942257</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>516.01s</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>22.69s</t>
-        </is>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="J10">
-        <f>K10*60+L10</f>
-        <v>109.97</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>49.969999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>111.69</v>
-      </c>
-      <c r="C11">
-        <f>$B$2/B11</f>
-        <v>3.6627271913331545</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>565.30s</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>24.69s</t>
-        </is>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="2">
-        <v>5.2800000000000002</v>
-      </c>
-      <c r="J11">
-        <f>K11*60+L11</f>
-        <v>111.69</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>51.689999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>111.11</v>
-      </c>
-      <c r="C12">
-        <f>$B$2/B12</f>
-        <v>3.681846818468185</v>
-      </c>
-      <c r="E12">
-        <v>11</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>608.05s</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>27.83s</t>
-        </is>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="2">
-        <v>5.7199999999999998</v>
-      </c>
-      <c r="J12">
-        <f>K12*60+L12</f>
-        <v>111.11</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>51.109999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>111.86</v>
-      </c>
-      <c r="C13">
-        <f>$B$2/B13</f>
-        <v>3.6571607366350798</v>
-      </c>
-      <c r="E13">
-        <v>12</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>657.91s</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>31.55s</t>
-        </is>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="2">
-        <v>6.1600000000000001</v>
-      </c>
-      <c r="J13">
-        <f>K13*60+L13</f>
-        <v>111.86</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>51.859999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>113.03</v>
-      </c>
-      <c r="C14">
-        <f>$B$2/B14</f>
-        <v>3.6193046093957357</v>
-      </c>
-      <c r="E14">
-        <v>13</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>699.08s</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>35.96s</t>
-        </is>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="J14">
-        <f>K14*60+L14</f>
-        <v>113.03</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>53.030000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>113.22</v>
-      </c>
-      <c r="C15">
-        <f>$B$2/B15</f>
-        <v>3.6132308779367608</v>
-      </c>
-      <c r="E15">
-        <v>14</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>742.17s</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>40.00s</t>
-        </is>
-      </c>
-      <c r="H15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="2">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="J15">
-        <f>K15*60+L15</f>
-        <v>113.22</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>53.219999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>114.89</v>
-      </c>
-      <c r="C16">
-        <f>$B$2/B16</f>
-        <v>3.5607102445817742</v>
-      </c>
-      <c r="E16">
-        <v>15</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>788.81s</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>45.20s</t>
-        </is>
-      </c>
-      <c r="H16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="2">
-        <v>7.25</v>
-      </c>
-      <c r="J16">
-        <f>K16*60+L16</f>
-        <v>114.89</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>54.890000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>115.74000000000001</v>
-      </c>
-      <c r="C17">
-        <f>$B$2/B17</f>
-        <v>3.5345602211854157</v>
-      </c>
-      <c r="E17">
-        <v>16</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>821.18s</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>52.66s</t>
-        </is>
-      </c>
-      <c r="H17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="2">
-        <v>7.54</v>
-      </c>
-      <c r="J17">
-        <f>K17*60+L17</f>
-        <v>115.74000000000001</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>55.740000000000002</v>
-      </c>
+        <v>4.139680483592401</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="I17" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
New benchmarks after caching
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>Total</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Default settings, but NUM_THREAD, OMP_NUM_THREAD set to 1</t>
+  </si>
+  <si>
+    <t>Default settings, after introducing caching</t>
   </si>
 </sst>
 </file>
@@ -119,36 +122,36 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:XFD36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" style="0" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" style="0" width="16.26953125" customWidth="1"/>
-    <col min="3" max="5" style="0" width="9.142307692307693"/>
+    <col min="3" max="5" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
     <col min="6" max="6" style="0" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" style="0" width="9.142307692307693"/>
+    <col min="7" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:16384">
       <c r="A1" t="inlineStr">
         <is>
           <t>Timings for running</t>
         </is>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:16384">
       <c r="A2" t="inlineStr">
         <is>
           <t>make benchmark</t>
         </is>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:16384">
       <c r="A4" t="inlineStr">
         <is>
           <t>Date</t>
@@ -193,7 +196,7 @@
         </is>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:16384">
       <c r="A5" s="1">
         <v>44497</v>
       </c>
@@ -221,7 +224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:16384">
       <c r="A6" s="1">
         <v>44497</v>
       </c>
@@ -249,7 +252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:16384">
       <c r="A7" s="1">
         <v>44497</v>
       </c>
@@ -282,7 +285,7 @@
         </is>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:16384">
       <c r="A8" s="1">
         <v>44498</v>
       </c>
@@ -313,7 +316,7 @@
         </is>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:16384">
       <c r="A9" s="1">
         <v>44498</v>
       </c>
@@ -344,7 +347,7 @@
         </is>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="13.5">
+    <row r="10" spans="1:16384" ht="13.5">
       <c r="A10" s="1">
         <v>44498</v>
       </c>
@@ -375,7 +378,7 @@
         </is>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:16384">
       <c r="A11" s="1">
         <v>44498</v>
       </c>
@@ -398,7 +401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:16384">
       <c r="A12" s="1">
         <v>44498</v>
       </c>
@@ -426,7 +429,7 @@
         </is>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:16384">
       <c r="A13" s="1">
         <v>44504</v>
       </c>
@@ -452,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="13.5">
+    <row r="14" spans="1:16384" ht="13.5">
       <c r="A14" s="1">
         <v>44505</v>
       </c>
@@ -483,7 +486,7 @@
         </is>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="13.5">
+    <row r="15" spans="1:16384" ht="13.5">
       <c r="A15" s="1">
         <v>44505</v>
       </c>
@@ -509,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:16384">
       <c r="A16" s="1">
         <v>44510</v>
       </c>
@@ -540,7 +543,7 @@
         </is>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:16384">
       <c r="A17" s="1">
         <v>44526</v>
       </c>
@@ -571,7 +574,7 @@
         </is>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:16384">
       <c r="A18" s="1">
         <v>44526</v>
       </c>
@@ -602,7 +605,7 @@
         </is>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:16384">
       <c r="A19" s="1">
         <v>44526</v>
       </c>
@@ -633,7 +636,7 @@
         </is>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:16384">
       <c r="A20" s="1">
         <v>44526</v>
       </c>
@@ -664,7 +667,7 @@
         </is>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:16384">
       <c r="A21" s="1">
         <v>44526</v>
       </c>
@@ -695,7 +698,7 @@
         </is>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:16384">
       <c r="A22" s="1">
         <v>44526</v>
       </c>
@@ -726,7 +729,7 @@
         </is>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:16384">
       <c r="A23" s="1">
         <v>44526</v>
       </c>
@@ -757,7 +760,7 @@
         </is>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="13.5">
+    <row r="24" spans="1:16384" ht="13.5">
       <c r="A24" s="1">
         <v>44518</v>
       </c>
@@ -780,7 +783,7 @@
         </is>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="13.5">
+    <row r="25" spans="1:16384" ht="13.5">
       <c r="A25" s="1">
         <v>44518</v>
       </c>
@@ -797,7 +800,7 @@
         </is>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:16384">
       <c r="A26" s="1">
         <v>44531</v>
       </c>
@@ -822,7 +825,7 @@
         </is>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="13.5">
+    <row r="27" spans="1:16384" ht="13.5">
       <c r="A27" s="1">
         <v>44518</v>
       </c>
@@ -845,7 +848,7 @@
         </is>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="13.5">
+    <row r="28" spans="1:16384" ht="13.5">
       <c r="A28" s="1">
         <v>44532</v>
       </c>
@@ -876,7 +879,7 @@
         </is>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="13.5">
+    <row r="29" spans="1:16384" ht="13.5">
       <c r="A29" s="1">
         <v>44532</v>
       </c>
@@ -907,7 +910,7 @@
         </is>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="13.5">
+    <row r="30" spans="1:16384" ht="13.5">
       <c r="A30" s="1">
         <v>44532</v>
       </c>
@@ -939,7 +942,7 @@
         </is>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5">
+    <row r="31" spans="1:16384" ht="13.5">
       <c r="A31" s="1">
         <v>44532</v>
       </c>
@@ -962,7 +965,7 @@
         </is>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="13.5">
+    <row r="32" spans="1:16384" ht="13.5">
       <c r="A32" s="1">
         <v>44532</v>
       </c>
@@ -985,7 +988,7 @@
         </is>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="13.5">
+    <row r="33" spans="1:16384" ht="13.5">
       <c r="A33" s="1">
         <v>44532</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="13.5">
+    <row r="34" spans="1:16384" ht="13.5">
       <c r="A34" s="1">
         <v>44532</v>
       </c>
@@ -1024,6 +1027,64 @@
       </c>
       <c r="L34" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16384" ht="15">
+      <c r="A35" s="1">
+        <v>44539</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>364.13999999999999</v>
+      </c>
+      <c r="D35">
+        <v>7.4199999999999999</v>
+      </c>
+      <c r="E35">
+        <v>307</v>
+      </c>
+      <c r="F35">
+        <v>120</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16384" ht="15">
+      <c r="A36" s="1">
+        <v>44539</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>332</v>
+      </c>
+      <c r="D36">
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="E36">
+        <v>347</v>
+      </c>
+      <c r="F36">
+        <v>97.400000000000006</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1043,20 +1104,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:XFD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" style="0" width="9.142307692307693"/>
+    <col min="1" max="2" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="0" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" style="0" width="9.142307692307693"/>
+    <col min="4" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:16384">
       <c r="A1" t="inlineStr">
         <is>
           <t>Processors</t>
@@ -1071,7 +1132,7 @@
         </is>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5">
+    <row r="2" spans="1:16384" ht="13.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1084,7 +1145,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="13.5">
+    <row r="3" spans="1:16384" ht="13.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1098,7 +1159,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="13.5">
+    <row r="4" spans="1:16384" ht="13.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1112,7 +1173,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="13.5">
+    <row r="5" spans="1:16384" ht="13.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1126,7 +1187,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="13.5">
+    <row r="6" spans="1:16384" ht="13.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1139,7 +1200,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5">
+    <row r="7" spans="1:16384" ht="13.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1152,7 +1213,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="13.5">
+    <row r="8" spans="1:16384" ht="13.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1165,7 +1226,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="13.5">
+    <row r="9" spans="1:16384" ht="13.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1178,28 +1239,28 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:16384">
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:16384">
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:16384">
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:16384">
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:16384">
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:16384">
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:16384">
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:16384">
       <c r="I17" s="2"/>
     </row>
   </sheetData>
@@ -1219,15 +1280,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Corrections to some of the API calls in the Helper examples Updated the benchmarks after some tuning
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="12800" windowHeight="8010"/>
+    <workbookView activeTab="0" windowWidth="19200" windowHeight="8320"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51" count="51">
+  <si>
+    <t>Timings for running</t>
+  </si>
+  <si>
+    <t>make benchmark</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>System%</t>
+  </si>
   <si>
     <t>Total</t>
   </si>
   <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>6.4.5</t>
+  </si>
+  <si>
     <t>Linux</t>
   </si>
   <si>
     <t>Intel core i9-9900K@3.6GHz</t>
   </si>
   <si>
+    <t>6.4.5 (develop)</t>
+  </si>
+  <si>
+    <t>6.4.3 (develop)</t>
+  </si>
+  <si>
+    <t>I was expecting this to be a lot quicker!</t>
+  </si>
+  <si>
     <t>7.0.1 (develop)</t>
   </si>
   <si>
+    <t>A bit better.</t>
+  </si>
+  <si>
+    <t>Removed excel checking</t>
+  </si>
+  <si>
+    <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
+  </si>
+  <si>
     <t>Windows</t>
   </si>
   <si>
     <t>Intel skylake (core m7) Intel Core(TM)i7-6500U@2.50GHz</t>
   </si>
   <si>
+    <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
+  </si>
+  <si>
+    <t>Running in a command shell</t>
+  </si>
+  <si>
+    <t>Getting ready to release</t>
+  </si>
+  <si>
+    <t>Switch from imap to map</t>
+  </si>
+  <si>
+    <t>Switching back to imap</t>
+  </si>
+  <si>
+    <t>Chunksize = 100</t>
+  </si>
+  <si>
+    <t>Chunksize = 20</t>
+  </si>
+  <si>
+    <t>Chunksize = 10</t>
+  </si>
+  <si>
+    <t>Chunksize = 5</t>
+  </si>
+  <si>
+    <t>Using new chunk sizes</t>
+  </si>
+  <si>
+    <t>Numthread=1, thread</t>
+  </si>
+  <si>
+    <t>Numthread=2, thread</t>
+  </si>
+  <si>
+    <t>Switched to multiprocessing (not pathos)</t>
+  </si>
+  <si>
+    <t>Using multiprocessing</t>
+  </si>
+  <si>
+    <t>Use partial method and removed crystal_permittivity array from call in powder</t>
+  </si>
+  <si>
+    <t>Replace readline with readlines and new io wrapper</t>
+  </si>
+  <si>
+    <t>Single processor</t>
+  </si>
+  <si>
+    <t>Default settings</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
+  </si>
+  <si>
     <t>Default settings, but NUM_THREAD, OMP_NUM_THREAD set to 1</t>
   </si>
   <si>
+    <t>8.1.1(develop)</t>
+  </si>
+  <si>
+    <t>Default settings, spending a lot time reading spread sheets</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_CORES=4</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_CORES=1</t>
+  </si>
+  <si>
     <t>Default settings, after introducing caching</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Processors</t>
+  </si>
+  <si>
+    <t>Speedup</t>
   </si>
 </sst>
 </file>
@@ -122,10 +251,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD36"/>
+  <dimension ref="A1:XFD40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
@@ -138,72 +267,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Timings for running</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:16384">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>make benchmark</t>
-        </is>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>User</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>System%</t>
-        </is>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>OS</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16384">
       <c r="A5" s="1">
         <v>44497</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>6.4.5</t>
-        </is>
+      <c r="B5" t="s">
+        <v>11</v>
       </c>
       <c r="C5">
         <v>885.27999999999997</v>
@@ -218,20 +325,18 @@
         <v>296.36000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="1">
         <v>44497</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6.4.5 (develop)</t>
-        </is>
+      <c r="B6" t="s">
+        <v>14</v>
       </c>
       <c r="C6">
         <v>874.24000000000001</v>
@@ -246,20 +351,18 @@
         <v>294.24000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" s="1">
         <v>44497</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>6.4.3 (develop)</t>
-        </is>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="C7">
         <v>720.80999999999995</v>
@@ -274,15 +377,13 @@
         <v>251.06</v>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>I was expecting this to be a lot quicker!</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:16384">
@@ -290,7 +391,7 @@
         <v>44498</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>589.29999999999995</v>
@@ -305,15 +406,13 @@
         <v>232.59</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>A bit better.</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16384">
@@ -321,7 +420,7 @@
         <v>44498</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>469.01999999999998</v>
@@ -336,15 +435,13 @@
         <v>107.65000000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Removed excel checking</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:16384" ht="13.5">
@@ -352,7 +449,7 @@
         <v>44498</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>599.09000000000003</v>
@@ -367,15 +464,13 @@
         <v>346.07999999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16384">
@@ -383,7 +478,7 @@
         <v>44498</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -395,10 +490,10 @@
         <v>1419.2529999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:16384">
@@ -406,7 +501,7 @@
         <v>44498</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -418,15 +513,13 @@
         <v>1104.95</v>
       </c>
       <c r="G12" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:16384">
@@ -434,7 +527,7 @@
         <v>44504</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>469.5</v>
@@ -449,10 +542,10 @@
         <v>110.23999999999999</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:16384" ht="13.5">
@@ -460,7 +553,7 @@
         <v>44505</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -475,15 +568,13 @@
         <v>1612</v>
       </c>
       <c r="G14" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Running in a command shell</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:16384" ht="13.5">
@@ -491,7 +582,7 @@
         <v>44505</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -506,10 +597,10 @@
         <v>1214</v>
       </c>
       <c r="G15" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:16384">
@@ -517,7 +608,7 @@
         <v>44510</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>465.02999999999997</v>
@@ -532,15 +623,13 @@
         <v>107.29000000000001</v>
       </c>
       <c r="G16" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Getting ready to release</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:16384">
@@ -548,7 +637,7 @@
         <v>44526</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>464.89999999999998</v>
@@ -563,15 +652,13 @@
         <v>110.62</v>
       </c>
       <c r="G17" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Switch from imap to map</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:16384">
@@ -579,7 +666,7 @@
         <v>44526</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>500.31</v>
@@ -594,15 +681,13 @@
         <v>115.90000000000001</v>
       </c>
       <c r="G18" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Switching back to imap</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:16384">
@@ -610,7 +695,7 @@
         <v>44526</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>450.25999999999999</v>
@@ -625,15 +710,13 @@
         <v>116</v>
       </c>
       <c r="G19" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Chunksize = 100</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:16384">
@@ -641,7 +724,7 @@
         <v>44526</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>485.97000000000003</v>
@@ -656,15 +739,13 @@
         <v>111.48999999999999</v>
       </c>
       <c r="G20" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Chunksize = 20</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:16384">
@@ -672,7 +753,7 @@
         <v>44526</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>490.81999999999999</v>
@@ -687,15 +768,13 @@
         <v>113.12</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Chunksize = 10</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:16384">
@@ -703,7 +782,7 @@
         <v>44526</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>532.49000000000001</v>
@@ -718,15 +797,13 @@
         <v>123.36</v>
       </c>
       <c r="G22" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>2</v>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Chunksize = 5</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:16384">
@@ -734,7 +811,7 @@
         <v>44526</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>619.51999999999998</v>
@@ -749,15 +826,13 @@
         <v>355.06999999999999</v>
       </c>
       <c r="G23" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Using new chunk sizes</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:16384" ht="13.5">
@@ -765,22 +840,20 @@
         <v>44518</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F24">
         <f>9*60+44</f>
         <v>584</v>
       </c>
       <c r="G24" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H24" t="s">
-        <v>5</v>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Numthread=1, thread</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:16384" ht="13.5">
@@ -788,16 +861,14 @@
         <v>44518</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F25">
         <f>19*60+41</f>
         <v>1181</v>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Numthread=2, thread</t>
-        </is>
+      <c r="L25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:16384">
@@ -805,7 +876,7 @@
         <v>44531</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C26">
         <v>419.43000000000001</v>
@@ -819,10 +890,8 @@
       <c r="F26">
         <v>100.3</v>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Switched to multiprocessing (not pathos)</t>
-        </is>
+      <c r="L26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:16384" ht="13.5">
@@ -830,22 +899,20 @@
         <v>44518</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F27">
         <f>16*60+23</f>
         <v>983</v>
       </c>
       <c r="G27" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H27" t="s">
-        <v>5</v>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Using multiprocessing</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:16384" ht="13.5">
@@ -853,7 +920,7 @@
         <v>44532</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>362.75</v>
@@ -868,15 +935,13 @@
         <v>96.400000000000006</v>
       </c>
       <c r="G28" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>2</v>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Use partial method and removed crystal_permittivity array from call in powder</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:16384" ht="13.5">
@@ -884,7 +949,7 @@
         <v>44532</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <v>344.39999999999998</v>
@@ -899,15 +964,13 @@
         <v>91.200000000000003</v>
       </c>
       <c r="G29" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>2</v>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Replace readline with readlines and new io wrapper</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L29" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:16384" ht="13.5">
@@ -915,7 +978,7 @@
         <v>44532</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C30">
         <v>399.45999999999998</v>
@@ -931,15 +994,13 @@
         <v>346</v>
       </c>
       <c r="G30" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>2</v>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Single processor</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="L30" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:16384" ht="13.5">
@@ -947,22 +1008,20 @@
         <v>44532</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F31">
         <f>7*60+30.109999999999999</f>
         <v>450.11000000000001</v>
       </c>
       <c r="G31" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>5</v>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Default settings</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:16384" ht="13.5">
@@ -970,22 +1029,20 @@
         <v>44532</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F32">
         <f>9*60+53</f>
         <v>593</v>
       </c>
       <c r="G32" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H32" t="s">
-        <v>5</v>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="L32" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:16384" ht="13.5">
@@ -993,20 +1050,20 @@
         <v>44532</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F33">
         <f>7*60+12</f>
         <v>432</v>
       </c>
       <c r="G33" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H33" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L33" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:16384" ht="13.5">
@@ -1014,77 +1071,171 @@
         <v>44532</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F34">
         <v>358.08999999999997</v>
       </c>
       <c r="G34" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L34" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:16384" ht="15">
       <c r="A35" s="1">
-        <v>44539</v>
+        <v>45475</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C35">
-        <v>364.13999999999999</v>
+        <v>428.62</v>
       </c>
       <c r="D35">
-        <v>7.4199999999999999</v>
+        <v>7.6500000000000004</v>
       </c>
       <c r="E35">
-        <v>307</v>
+        <v>250</v>
       </c>
       <c r="F35">
-        <v>120</v>
+        <v>174.286</v>
       </c>
       <c r="G35" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="L35" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:16384" ht="15">
       <c r="A36" s="1">
+        <v>45475</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36">
+        <v>390.93000000000001</v>
+      </c>
+      <c r="D36">
+        <v>6.5</v>
+      </c>
+      <c r="E36">
+        <v>199</v>
+      </c>
+      <c r="F36">
+        <v>199.47999999999999</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16384" ht="15">
+      <c r="A37" s="1">
+        <v>45475</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>404.44</v>
+      </c>
+      <c r="D37">
+        <v>8.3399999999999999</v>
+      </c>
+      <c r="E37">
+        <v>104</v>
+      </c>
+      <c r="F37">
+        <v>394.72000000000003</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16384" ht="15">
+      <c r="A38" s="1">
         <v>44539</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>364.13999999999999</v>
+      </c>
+      <c r="D38">
+        <v>7.4199999999999999</v>
+      </c>
+      <c r="E38">
+        <v>307</v>
+      </c>
+      <c r="F38">
+        <v>120</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16384" ht="15">
+      <c r="A39" s="1">
+        <v>44539</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
         <v>332</v>
       </c>
-      <c r="D36">
+      <c r="D39">
         <v>7.2999999999999998</v>
       </c>
-      <c r="E36">
+      <c r="E39">
         <v>347</v>
       </c>
-      <c r="F36">
+      <c r="F39">
         <v>97.400000000000006</v>
       </c>
-      <c r="G36" t="s">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>5</v>
-      </c>
-      <c r="L36" t="s">
-        <v>7</v>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Default settings, after introducing caching and not closing database</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:16384" ht="15">
+      <c r="L40" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1118,18 +1269,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Processors</t>
-        </is>
+      <c r="A1" t="s">
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Speedup</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:16384" ht="13.5">

</xml_diff>

<commit_message>
New benchmark result for an AMD mobile processor on Linux
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="19200" windowHeight="8320"/>
+    <workbookView activeTab="0" windowWidth="14400" windowHeight="6250"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -25,42 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51" count="51">
-  <si>
-    <t>Timings for running</t>
-  </si>
-  <si>
-    <t>make benchmark</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>System%</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>Machine</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>6.4.5</t>
   </si>
   <si>
     <t>Linux</t>
@@ -69,25 +36,7 @@
     <t>Intel core i9-9900K@3.6GHz</t>
   </si>
   <si>
-    <t>6.4.5 (develop)</t>
-  </si>
-  <si>
-    <t>6.4.3 (develop)</t>
-  </si>
-  <si>
-    <t>I was expecting this to be a lot quicker!</t>
-  </si>
-  <si>
     <t>7.0.1 (develop)</t>
-  </si>
-  <si>
-    <t>A bit better.</t>
-  </si>
-  <si>
-    <t>Removed excel checking</t>
-  </si>
-  <si>
-    <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
   </si>
   <si>
     <t>Windows</t>
@@ -96,88 +45,13 @@
     <t>Intel skylake (core m7) Intel Core(TM)i7-6500U@2.50GHz</t>
   </si>
   <si>
-    <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
-  </si>
-  <si>
-    <t>Running in a command shell</t>
-  </si>
-  <si>
-    <t>Getting ready to release</t>
-  </si>
-  <si>
-    <t>Switch from imap to map</t>
-  </si>
-  <si>
-    <t>Switching back to imap</t>
-  </si>
-  <si>
-    <t>Chunksize = 100</t>
-  </si>
-  <si>
-    <t>Chunksize = 20</t>
-  </si>
-  <si>
-    <t>Chunksize = 10</t>
-  </si>
-  <si>
-    <t>Chunksize = 5</t>
-  </si>
-  <si>
-    <t>Using new chunk sizes</t>
-  </si>
-  <si>
-    <t>Numthread=1, thread</t>
-  </si>
-  <si>
-    <t>Numthread=2, thread</t>
-  </si>
-  <si>
-    <t>Switched to multiprocessing (not pathos)</t>
-  </si>
-  <si>
-    <t>Using multiprocessing</t>
-  </si>
-  <si>
-    <t>Use partial method and removed crystal_permittivity array from call in powder</t>
-  </si>
-  <si>
-    <t>Replace readline with readlines and new io wrapper</t>
-  </si>
-  <si>
-    <t>Single processor</t>
-  </si>
-  <si>
     <t>Default settings</t>
-  </si>
-  <si>
-    <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
   </si>
   <si>
     <t>Default settings, but NUM_THREAD, OMP_NUM_THREAD set to 1</t>
   </si>
   <si>
     <t>8.1.1(develop)</t>
-  </si>
-  <si>
-    <t>Default settings, spending a lot time reading spread sheets</t>
-  </si>
-  <si>
-    <t>PDIELEC_NUM_CORES=4</t>
-  </si>
-  <si>
-    <t>PDIELEC_NUM_CORES=1</t>
-  </si>
-  <si>
-    <t>Default settings, after introducing caching</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Processors</t>
-  </si>
-  <si>
-    <t>Speedup</t>
   </si>
 </sst>
 </file>
@@ -253,13 +127,13 @@
   </sheetPr>
   <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView topLeftCell="A18" workbookViewId="0" tabSelected="1">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" style="0" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="0" width="21.427283653846157" customWidth="1"/>
     <col min="2" max="2" style="0" width="16.26953125" customWidth="1"/>
     <col min="3" max="5" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
     <col min="6" max="6" style="0" width="9.26953125" bestFit="1" customWidth="1"/>
@@ -267,50 +141,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
-      <c r="A1" t="s">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Timings for running</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:16384">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>make benchmark</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:16384">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>System%</t>
+        </is>
+      </c>
+      <c r="F4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:16384">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16384">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>OS</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Machine</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
       </c>
     </row>
     <row r="5" spans="1:16384">
       <c r="A5" s="1">
         <v>44497</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6.4.5</t>
+        </is>
       </c>
       <c r="C5">
         <v>885.27999999999997</v>
@@ -325,18 +221,20 @@
         <v>296.36000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="1">
         <v>44497</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6.4.5 (develop)</t>
+        </is>
       </c>
       <c r="C6">
         <v>874.24000000000001</v>
@@ -351,18 +249,20 @@
         <v>294.24000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" s="1">
         <v>44497</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6.4.3 (develop)</t>
+        </is>
       </c>
       <c r="C7">
         <v>720.80999999999995</v>
@@ -377,13 +277,15 @@
         <v>251.06</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>I was expecting this to be a lot quicker!</t>
+        </is>
       </c>
     </row>
     <row r="8" spans="1:16384">
@@ -391,7 +293,7 @@
         <v>44498</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>589.29999999999995</v>
@@ -406,13 +308,15 @@
         <v>232.59</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>A bit better.</t>
+        </is>
       </c>
     </row>
     <row r="9" spans="1:16384">
@@ -420,7 +324,7 @@
         <v>44498</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>469.01999999999998</v>
@@ -435,13 +339,15 @@
         <v>107.65000000000001</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Removed excel checking</t>
+        </is>
       </c>
     </row>
     <row r="10" spans="1:16384" ht="13.5">
@@ -449,7 +355,7 @@
         <v>44498</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>599.09000000000003</v>
@@ -464,13 +370,15 @@
         <v>346.07999999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
+        </is>
       </c>
     </row>
     <row r="11" spans="1:16384">
@@ -478,7 +386,7 @@
         <v>44498</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -490,10 +398,10 @@
         <v>1419.2529999999999</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16384">
@@ -501,7 +409,7 @@
         <v>44498</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -513,13 +421,15 @@
         <v>1104.95</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
+        </is>
       </c>
     </row>
     <row r="13" spans="1:16384">
@@ -527,7 +437,7 @@
         <v>44504</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>469.5</v>
@@ -542,10 +452,10 @@
         <v>110.23999999999999</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:16384" ht="13.5">
@@ -553,7 +463,7 @@
         <v>44505</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -568,13 +478,15 @@
         <v>1612</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" t="s">
-        <v>24</v>
+        <v>5</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Running in a command shell</t>
+        </is>
       </c>
     </row>
     <row r="15" spans="1:16384" ht="13.5">
@@ -582,7 +494,7 @@
         <v>44505</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -597,10 +509,10 @@
         <v>1214</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16384">
@@ -608,7 +520,7 @@
         <v>44510</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>465.02999999999997</v>
@@ -623,13 +535,15 @@
         <v>107.29000000000001</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Getting ready to release</t>
+        </is>
       </c>
     </row>
     <row r="17" spans="1:16384">
@@ -637,7 +551,7 @@
         <v>44526</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>464.89999999999998</v>
@@ -652,13 +566,15 @@
         <v>110.62</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Switch from imap to map</t>
+        </is>
       </c>
     </row>
     <row r="18" spans="1:16384">
@@ -666,7 +582,7 @@
         <v>44526</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>500.31</v>
@@ -681,13 +597,15 @@
         <v>115.90000000000001</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Switching back to imap</t>
+        </is>
       </c>
     </row>
     <row r="19" spans="1:16384">
@@ -695,7 +613,7 @@
         <v>44526</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>450.25999999999999</v>
@@ -710,13 +628,15 @@
         <v>116</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Chunksize = 100</t>
+        </is>
       </c>
     </row>
     <row r="20" spans="1:16384">
@@ -724,7 +644,7 @@
         <v>44526</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>485.97000000000003</v>
@@ -739,13 +659,15 @@
         <v>111.48999999999999</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Chunksize = 20</t>
+        </is>
       </c>
     </row>
     <row r="21" spans="1:16384">
@@ -753,7 +675,7 @@
         <v>44526</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>490.81999999999999</v>
@@ -768,13 +690,15 @@
         <v>113.12</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Chunksize = 10</t>
+        </is>
       </c>
     </row>
     <row r="22" spans="1:16384">
@@ -782,7 +706,7 @@
         <v>44526</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>532.49000000000001</v>
@@ -797,13 +721,15 @@
         <v>123.36</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Chunksize = 5</t>
+        </is>
       </c>
     </row>
     <row r="23" spans="1:16384">
@@ -811,7 +737,7 @@
         <v>44526</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>619.51999999999998</v>
@@ -826,13 +752,15 @@
         <v>355.06999999999999</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Using new chunk sizes</t>
+        </is>
       </c>
     </row>
     <row r="24" spans="1:16384" ht="13.5">
@@ -840,20 +768,22 @@
         <v>44518</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F24">
         <f>9*60+44</f>
         <v>584</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Numthread=1, thread</t>
+        </is>
       </c>
     </row>
     <row r="25" spans="1:16384" ht="13.5">
@@ -861,14 +791,16 @@
         <v>44518</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F25">
         <f>19*60+41</f>
         <v>1181</v>
       </c>
-      <c r="L25" t="s">
-        <v>34</v>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Numthread=2, thread</t>
+        </is>
       </c>
     </row>
     <row r="26" spans="1:16384">
@@ -876,7 +808,7 @@
         <v>44531</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>419.43000000000001</v>
@@ -890,8 +822,10 @@
       <c r="F26">
         <v>100.3</v>
       </c>
-      <c r="L26" t="s">
-        <v>35</v>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Switched to multiprocessing (not pathos)</t>
+        </is>
       </c>
     </row>
     <row r="27" spans="1:16384" ht="13.5">
@@ -899,20 +833,22 @@
         <v>44518</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F27">
         <f>16*60+23</f>
         <v>983</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Using multiprocessing</t>
+        </is>
       </c>
     </row>
     <row r="28" spans="1:16384" ht="13.5">
@@ -920,7 +856,7 @@
         <v>44532</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>362.75</v>
@@ -935,13 +871,15 @@
         <v>96.400000000000006</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Use partial method and removed crystal_permittivity array from call in powder</t>
+        </is>
       </c>
     </row>
     <row r="29" spans="1:16384" ht="13.5">
@@ -949,7 +887,7 @@
         <v>44532</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>344.39999999999998</v>
@@ -964,13 +902,15 @@
         <v>91.200000000000003</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L29" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Replace readline with readlines and new io wrapper</t>
+        </is>
       </c>
     </row>
     <row r="30" spans="1:16384" ht="13.5">
@@ -978,7 +918,7 @@
         <v>44532</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>399.45999999999998</v>
@@ -994,13 +934,15 @@
         <v>346</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Single processor</t>
+        </is>
       </c>
     </row>
     <row r="31" spans="1:16384" ht="13.5">
@@ -1008,20 +950,20 @@
         <v>44532</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F31">
         <f>7*60+30.109999999999999</f>
         <v>450.11000000000001</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="L31" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:16384" ht="13.5">
@@ -1029,20 +971,22 @@
         <v>44532</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F32">
         <f>9*60+53</f>
         <v>593</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" t="s">
-        <v>41</v>
+        <v>5</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
+        </is>
       </c>
     </row>
     <row r="33" spans="1:16384" ht="13.5">
@@ -1050,20 +994,20 @@
         <v>44532</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <f>7*60+12</f>
         <v>432</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="L33" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:16384" ht="13.5">
@@ -1071,19 +1015,19 @@
         <v>44532</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F34">
         <v>358.08999999999997</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="L34" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:16384" ht="15">
@@ -1091,7 +1035,7 @@
         <v>45475</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>428.62</v>
@@ -1106,13 +1050,15 @@
         <v>174.286</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
-      </c>
-      <c r="L35" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Default settings, spending a lot time reading spread sheets</t>
+        </is>
       </c>
     </row>
     <row r="36" spans="1:16384" ht="15">
@@ -1120,7 +1066,7 @@
         <v>45475</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>390.93000000000001</v>
@@ -1135,13 +1081,15 @@
         <v>199.47999999999999</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L36" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>PDIELEC_NUM_CORES=4</t>
+        </is>
       </c>
     </row>
     <row r="37" spans="1:16384" ht="15">
@@ -1149,7 +1097,7 @@
         <v>45475</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <v>404.44</v>
@@ -1164,13 +1112,15 @@
         <v>394.72000000000003</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="L37" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>PDIELEC_NUM_CORES=1</t>
+        </is>
       </c>
     </row>
     <row r="38" spans="1:16384" ht="15">
@@ -1178,7 +1128,7 @@
         <v>44539</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>364.13999999999999</v>
@@ -1193,13 +1143,15 @@
         <v>120</v>
       </c>
       <c r="G38" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>13</v>
-      </c>
-      <c r="L38" t="s">
-        <v>47</v>
+        <v>2</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Default settings, after introducing caching</t>
+        </is>
       </c>
     </row>
     <row r="39" spans="1:16384" ht="15">
@@ -1207,7 +1159,7 @@
         <v>44539</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>332</v>
@@ -1222,10 +1174,10 @@
         <v>97.400000000000006</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
@@ -1234,8 +1186,36 @@
       </c>
     </row>
     <row r="40" spans="1:16384" ht="15">
+      <c r="A40" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>8.1.3 (develop)</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>430</v>
+      </c>
+      <c r="D40">
+        <v>13.66</v>
+      </c>
+      <c r="E40">
+        <v>366</v>
+      </c>
+      <c r="F40">
+        <v>121</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>AMD Ryzen 7 5700U with Radeon Graphics</t>
+        </is>
+      </c>
       <c r="L40" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1269,14 +1249,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
-      <c r="A1" t="s">
-        <v>49</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Processors</t>
+        </is>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Speedup</t>
+        </is>
       </c>
     </row>
     <row r="2" spans="1:16384" ht="13.5">

</xml_diff>

<commit_message>
Updated benchmarks for Windows Notebook
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\PDielec\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40EF360-92D3-458C-9BDD-E6BB4A087A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="6250"/>
+    <workbookView xWindow="10935" yWindow="3975" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -12,20 +18,20 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="191029" iterate="1"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>Total</t>
   </si>
@@ -52,25 +58,155 @@
   </si>
   <si>
     <t>8.1.1(develop)</t>
+  </si>
+  <si>
+    <t>Timings for running</t>
+  </si>
+  <si>
+    <t>make benchmark</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>System%</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>6.4.5</t>
+  </si>
+  <si>
+    <t>6.4.5 (develop)</t>
+  </si>
+  <si>
+    <t>6.4.3 (develop)</t>
+  </si>
+  <si>
+    <t>I was expecting this to be a lot quicker!</t>
+  </si>
+  <si>
+    <t>A bit better.</t>
+  </si>
+  <si>
+    <t>Removed excel checking</t>
+  </si>
+  <si>
+    <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
+  </si>
+  <si>
+    <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
+  </si>
+  <si>
+    <t>Running in a command shell</t>
+  </si>
+  <si>
+    <t>Getting ready to release</t>
+  </si>
+  <si>
+    <t>Switch from imap to map</t>
+  </si>
+  <si>
+    <t>Switching back to imap</t>
+  </si>
+  <si>
+    <t>Chunksize = 100</t>
+  </si>
+  <si>
+    <t>Chunksize = 20</t>
+  </si>
+  <si>
+    <t>Chunksize = 10</t>
+  </si>
+  <si>
+    <t>Chunksize = 5</t>
+  </si>
+  <si>
+    <t>Using new chunk sizes</t>
+  </si>
+  <si>
+    <t>Numthread=1, thread</t>
+  </si>
+  <si>
+    <t>Numthread=2, thread</t>
+  </si>
+  <si>
+    <t>Switched to multiprocessing (not pathos)</t>
+  </si>
+  <si>
+    <t>Using multiprocessing</t>
+  </si>
+  <si>
+    <t>Use partial method and removed crystal_permittivity array from call in powder</t>
+  </si>
+  <si>
+    <t>Replace readline with readlines and new io wrapper</t>
+  </si>
+  <si>
+    <t>Single processor</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
+  </si>
+  <si>
+    <t>Default settings, spending a lot time reading spread sheets</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_CORES=4</t>
+  </si>
+  <si>
+    <t>Default settings, after introducing caching</t>
+  </si>
+  <si>
+    <t>Default settings, after introducing caching and not closing database</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 5700U with Radeon Graphics</t>
+  </si>
+  <si>
+    <t>Processors</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>8.1.3 (QT6)</t>
+  </si>
+  <si>
+    <t>PDIELEC_NUM_PROCESSORS=1</t>
+  </si>
+  <si>
+    <t>Num Processors =1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt formatCode="d/m/yyyy" numFmtId="100"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,143 +218,428 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:XFD40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="21.427283653846157" customWidth="1"/>
-    <col min="2" max="2" style="0" width="16.26953125" customWidth="1"/>
-    <col min="3" max="5" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" style="0" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Timings for running</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:16384">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>make benchmark</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" spans="1:16384">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>User</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>System%</t>
-        </is>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>OS</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" spans="1:16384">
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>44497</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>6.4.5</t>
-        </is>
+      <c r="B5" t="s">
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>885.27999999999997</v>
+        <v>885.28</v>
       </c>
       <c r="D5">
-        <v>33.240000000000002</v>
+        <v>33.24</v>
       </c>
       <c r="E5">
         <v>309</v>
       </c>
       <c r="F5">
-        <v>296.36000000000001</v>
+        <v>296.36</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -227,26 +648,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>44497</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6.4.5 (develop)</t>
-        </is>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>874.24000000000001</v>
+        <v>874.24</v>
       </c>
       <c r="D6">
-        <v>32.890000000000001</v>
+        <v>32.89</v>
       </c>
       <c r="E6">
         <v>308</v>
       </c>
       <c r="F6">
-        <v>294.24000000000001</v>
+        <v>294.24</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -255,20 +674,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>44497</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>6.4.3 (develop)</t>
-        </is>
+      <c r="B7" t="s">
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>720.80999999999995</v>
+        <v>720.81</v>
       </c>
       <c r="D7">
-        <v>30.940000000000001</v>
+        <v>30.94</v>
       </c>
       <c r="E7">
         <v>299</v>
@@ -282,13 +699,11 @@
       <c r="H7" t="s">
         <v>2</v>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>I was expecting this to be a lot quicker!</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" spans="1:16384">
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>44498</v>
       </c>
@@ -299,7 +714,7 @@
         <v>589.29999999999995</v>
       </c>
       <c r="D8">
-        <v>20.829999999999998</v>
+        <v>20.83</v>
       </c>
       <c r="E8">
         <v>262</v>
@@ -313,13 +728,11 @@
       <c r="H8" t="s">
         <v>2</v>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>A bit better.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" spans="1:16384">
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>44498</v>
       </c>
@@ -327,16 +740,16 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>469.01999999999998</v>
+        <v>469.02</v>
       </c>
       <c r="D9">
-        <v>19.469999999999999</v>
+        <v>19.47</v>
       </c>
       <c r="E9">
         <v>453</v>
       </c>
       <c r="F9">
-        <v>107.65000000000001</v>
+        <v>107.65</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
@@ -344,13 +757,11 @@
       <c r="H9" t="s">
         <v>2</v>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Removed excel checking</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" spans="1:16384" ht="13.5">
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>44498</v>
       </c>
@@ -358,16 +769,16 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>599.09000000000003</v>
+        <v>599.09</v>
       </c>
       <c r="D10">
-        <v>11.529999999999999</v>
+        <v>11.53</v>
       </c>
       <c r="E10">
         <v>176</v>
       </c>
       <c r="F10">
-        <v>346.07999999999998</v>
+        <v>346.08</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
@@ -375,13 +786,11 @@
       <c r="H10" t="s">
         <v>2</v>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Need to make sure only 1 thread was used for BLAS and for OMP</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" spans="1:16384">
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>44498</v>
       </c>
@@ -404,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>44498</v>
       </c>
@@ -426,13 +835,11 @@
       <c r="H12" t="s">
         <v>5</v>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Added Num_THREAD=1 and OMP_NUM_THREAD=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" spans="1:16384">
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>44504</v>
       </c>
@@ -443,13 +850,13 @@
         <v>469.5</v>
       </c>
       <c r="D13">
-        <v>20.219999999999999</v>
+        <v>20.22</v>
       </c>
       <c r="E13">
         <v>444</v>
       </c>
       <c r="F13">
-        <v>110.23999999999999</v>
+        <v>110.24</v>
       </c>
       <c r="G13" t="s">
         <v>1</v>
@@ -458,7 +865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" ht="13.5">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>44505</v>
       </c>
@@ -483,13 +890,11 @@
       <c r="H14" t="s">
         <v>5</v>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Running in a command shell</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" spans="1:16384" ht="13.5">
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>44505</v>
       </c>
@@ -515,7 +920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16384">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>44510</v>
       </c>
@@ -523,16 +928,16 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>465.02999999999997</v>
+        <v>465.03</v>
       </c>
       <c r="D16">
-        <v>19.629999999999999</v>
+        <v>19.63</v>
       </c>
       <c r="E16">
         <v>451</v>
       </c>
       <c r="F16">
-        <v>107.29000000000001</v>
+        <v>107.29</v>
       </c>
       <c r="G16" t="s">
         <v>1</v>
@@ -540,13 +945,11 @@
       <c r="H16" t="s">
         <v>2</v>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Getting ready to release</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" spans="1:16384">
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>44526</v>
       </c>
@@ -554,10 +957,10 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>464.89999999999998</v>
+        <v>464.9</v>
       </c>
       <c r="D17">
-        <v>15.609999999999999</v>
+        <v>15.61</v>
       </c>
       <c r="E17">
         <v>434</v>
@@ -571,13 +974,11 @@
       <c r="H17" t="s">
         <v>2</v>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Switch from imap to map</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" spans="1:16384">
+      <c r="L17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>44526</v>
       </c>
@@ -588,13 +989,13 @@
         <v>500.31</v>
       </c>
       <c r="D18">
-        <v>16.879999999999999</v>
+        <v>16.88</v>
       </c>
       <c r="E18">
         <v>445</v>
       </c>
       <c r="F18">
-        <v>115.90000000000001</v>
+        <v>115.9</v>
       </c>
       <c r="G18" t="s">
         <v>1</v>
@@ -602,13 +1003,11 @@
       <c r="H18" t="s">
         <v>2</v>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Switching back to imap</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" spans="1:16384">
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>44526</v>
       </c>
@@ -616,10 +1015,10 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>450.25999999999999</v>
+        <v>450.26</v>
       </c>
       <c r="D19">
-        <v>15.960000000000001</v>
+        <v>15.96</v>
       </c>
       <c r="E19">
         <v>401</v>
@@ -633,13 +1032,11 @@
       <c r="H19" t="s">
         <v>2</v>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Chunksize = 100</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" spans="1:16384">
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>44526</v>
       </c>
@@ -647,16 +1044,16 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>485.97000000000003</v>
+        <v>485.97</v>
       </c>
       <c r="D20">
-        <v>16.629999999999999</v>
+        <v>16.63</v>
       </c>
       <c r="E20">
         <v>450</v>
       </c>
       <c r="F20">
-        <v>111.48999999999999</v>
+        <v>111.49</v>
       </c>
       <c r="G20" t="s">
         <v>1</v>
@@ -664,13 +1061,11 @@
       <c r="H20" t="s">
         <v>2</v>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Chunksize = 20</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" spans="1:16384">
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>44526</v>
       </c>
@@ -678,10 +1073,10 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>490.81999999999999</v>
+        <v>490.82</v>
       </c>
       <c r="D21">
-        <v>18.460000000000001</v>
+        <v>18.46</v>
       </c>
       <c r="E21">
         <v>450</v>
@@ -695,13 +1090,11 @@
       <c r="H21" t="s">
         <v>2</v>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Chunksize = 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" spans="1:16384">
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>44526</v>
       </c>
@@ -709,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>532.49000000000001</v>
+        <v>532.49</v>
       </c>
       <c r="D22">
         <v>19.66</v>
@@ -726,13 +1119,11 @@
       <c r="H22" t="s">
         <v>2</v>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Chunksize = 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" spans="1:16384">
+      <c r="L22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>44526</v>
       </c>
@@ -740,16 +1131,16 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>619.51999999999998</v>
+        <v>619.52</v>
       </c>
       <c r="D23">
-        <v>11.359999999999999</v>
+        <v>11.36</v>
       </c>
       <c r="E23">
         <v>177</v>
       </c>
       <c r="F23">
-        <v>355.06999999999999</v>
+        <v>355.07</v>
       </c>
       <c r="G23" t="s">
         <v>1</v>
@@ -757,13 +1148,11 @@
       <c r="H23" t="s">
         <v>5</v>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Using new chunk sizes</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" spans="1:16384" ht="13.5">
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>44518</v>
       </c>
@@ -780,13 +1169,11 @@
       <c r="H24" t="s">
         <v>5</v>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Numthread=1, thread</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" spans="1:16384" ht="13.5">
+      <c r="L24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>44518</v>
       </c>
@@ -797,13 +1184,11 @@
         <f>19*60+41</f>
         <v>1181</v>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Numthread=2, thread</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" spans="1:16384">
+      <c r="L25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>44531</v>
       </c>
@@ -811,10 +1196,10 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>419.43000000000001</v>
+        <v>419.43</v>
       </c>
       <c r="D26">
-        <v>15.880000000000001</v>
+        <v>15.88</v>
       </c>
       <c r="E26">
         <v>433</v>
@@ -822,13 +1207,11 @@
       <c r="F26">
         <v>100.3</v>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Switched to multiprocessing (not pathos)</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" spans="1:16384" ht="13.5">
+      <c r="L26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>44518</v>
       </c>
@@ -845,13 +1228,11 @@
       <c r="H27" t="s">
         <v>5</v>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Using multiprocessing</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" spans="1:16384" ht="13.5">
+      <c r="L27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>44532</v>
       </c>
@@ -862,13 +1243,13 @@
         <v>362.75</v>
       </c>
       <c r="D28">
-        <v>6.2199999999999998</v>
+        <v>6.22</v>
       </c>
       <c r="E28">
         <v>382</v>
       </c>
       <c r="F28">
-        <v>96.400000000000006</v>
+        <v>96.4</v>
       </c>
       <c r="G28" t="s">
         <v>1</v>
@@ -876,13 +1257,11 @@
       <c r="H28" t="s">
         <v>2</v>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Use partial method and removed crystal_permittivity array from call in powder</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" spans="1:16384" ht="13.5">
+      <c r="L28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>44532</v>
       </c>
@@ -890,16 +1269,16 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>344.39999999999998</v>
+        <v>344.4</v>
       </c>
       <c r="D29">
-        <v>5.5800000000000001</v>
+        <v>5.58</v>
       </c>
       <c r="E29">
         <v>380</v>
       </c>
       <c r="F29">
-        <v>91.200000000000003</v>
+        <v>91.2</v>
       </c>
       <c r="G29" t="s">
         <v>1</v>
@@ -907,13 +1286,11 @@
       <c r="H29" t="s">
         <v>2</v>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Replace readline with readlines and new io wrapper</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" spans="1:16384" ht="13.5">
+      <c r="L29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>44532</v>
       </c>
@@ -921,10 +1298,10 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>399.45999999999998</v>
+        <v>399.46</v>
       </c>
       <c r="D30">
-        <v>38.240000000000002</v>
+        <v>38.24</v>
       </c>
       <c r="E30">
         <v>126</v>
@@ -939,13 +1316,11 @@
       <c r="H30" t="s">
         <v>2</v>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Single processor</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" spans="1:16384" ht="13.5">
+      <c r="L30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>44532</v>
       </c>
@@ -953,8 +1328,8 @@
         <v>3</v>
       </c>
       <c r="F31">
-        <f>7*60+30.109999999999999</f>
-        <v>450.11000000000001</v>
+        <f>7*60+30.1099999999999</f>
+        <v>450.1099999999999</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -966,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:16384" ht="13.5">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>44532</v>
       </c>
@@ -983,13 +1358,11 @@
       <c r="H32" t="s">
         <v>5</v>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>PDIELEC_NUM_THREAD=1, PDIELEC_NUM_CORES=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" spans="1:16384" ht="13.5">
+      <c r="L32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>44532</v>
       </c>
@@ -1010,7 +1383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:16384" ht="13.5">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>44532</v>
       </c>
@@ -1018,7 +1391,7 @@
         <v>3</v>
       </c>
       <c r="F34">
-        <v>358.08999999999997</v>
+        <v>358.09</v>
       </c>
       <c r="G34" t="s">
         <v>1</v>
@@ -1030,7 +1403,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" ht="15">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>45475</v>
       </c>
@@ -1041,7 +1414,7 @@
         <v>428.62</v>
       </c>
       <c r="D35">
-        <v>7.6500000000000004</v>
+        <v>7.65</v>
       </c>
       <c r="E35">
         <v>250</v>
@@ -1055,13 +1428,11 @@
       <c r="H35" t="s">
         <v>2</v>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>Default settings, spending a lot time reading spread sheets</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" spans="1:16384" ht="15">
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>45475</v>
       </c>
@@ -1069,7 +1440,7 @@
         <v>8</v>
       </c>
       <c r="C36">
-        <v>390.93000000000001</v>
+        <v>390.93</v>
       </c>
       <c r="D36">
         <v>6.5</v>
@@ -1078,7 +1449,7 @@
         <v>199</v>
       </c>
       <c r="F36">
-        <v>199.47999999999999</v>
+        <v>199.48</v>
       </c>
       <c r="G36" t="s">
         <v>1</v>
@@ -1086,13 +1457,11 @@
       <c r="H36" t="s">
         <v>2</v>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>PDIELEC_NUM_CORES=4</t>
-        </is>
-      </c>
-    </row>
-    <row r="37" spans="1:16384" ht="15">
+      <c r="L36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>45475</v>
       </c>
@@ -1103,13 +1472,13 @@
         <v>404.44</v>
       </c>
       <c r="D37">
-        <v>8.3399999999999999</v>
+        <v>8.34</v>
       </c>
       <c r="E37">
         <v>104</v>
       </c>
       <c r="F37">
-        <v>394.72000000000003</v>
+        <v>394.72</v>
       </c>
       <c r="G37" t="s">
         <v>1</v>
@@ -1117,13 +1486,11 @@
       <c r="H37" t="s">
         <v>2</v>
       </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>PDIELEC_NUM_CORES=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" spans="1:16384" ht="15">
+      <c r="L37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>44539</v>
       </c>
@@ -1131,10 +1498,10 @@
         <v>3</v>
       </c>
       <c r="C38">
-        <v>364.13999999999999</v>
+        <v>364.14</v>
       </c>
       <c r="D38">
-        <v>7.4199999999999999</v>
+        <v>7.42</v>
       </c>
       <c r="E38">
         <v>307</v>
@@ -1148,13 +1515,11 @@
       <c r="H38" t="s">
         <v>2</v>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Default settings, after introducing caching</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" spans="1:16384" ht="15">
+      <c r="L38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>44539</v>
       </c>
@@ -1165,13 +1530,13 @@
         <v>332</v>
       </c>
       <c r="D39">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="E39">
         <v>347</v>
       </c>
       <c r="F39">
-        <v>97.400000000000006</v>
+        <v>97.4</v>
       </c>
       <c r="G39" t="s">
         <v>1</v>
@@ -1179,20 +1544,16 @@
       <c r="H39" t="s">
         <v>2</v>
       </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Default settings, after introducing caching and not closing database</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" spans="1:16384" ht="15">
+      <c r="L39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>45531</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>8.1.3 (develop)</t>
-        </is>
+      <c r="B40" t="s">
+        <v>51</v>
       </c>
       <c r="C40">
         <v>430</v>
@@ -1209,20 +1570,86 @@
       <c r="G40" t="s">
         <v>1</v>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>AMD Ryzen 7 5700U with Radeon Graphics</t>
-        </is>
+      <c r="H40" t="s">
+        <v>48</v>
       </c>
       <c r="L40" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41">
+        <v>480</v>
+      </c>
+      <c r="F41">
+        <v>480</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>48</v>
+      </c>
+      <c r="L41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42">
+        <v>480</v>
+      </c>
+      <c r="F42">
+        <v>480</v>
+      </c>
+      <c r="G42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>48</v>
+      </c>
+      <c r="L42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43">
+        <v>988</v>
+      </c>
+      <c r="F43">
+        <v>988</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>48</v>
+      </c>
+      <c r="L43" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1231,39 +1658,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" style="0" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Processors</t>
-        </is>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Speedup</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:16384" ht="13.5">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1274,37 +1694,34 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:16384" ht="13.5">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f>3*60+5.2999999999999998</f>
-        <v>185.30000000000001</v>
+        <f>3*60+5.29999999999999</f>
+        <v>185.29999999999998</v>
       </c>
       <c r="C3">
-        <f>$B$2/B3</f>
-        <v>2.0696168375607122</v>
-      </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:16384" ht="13.5">
+        <f t="shared" ref="C3:C9" si="0">$B$2/B3</f>
+        <v>2.0696168375607127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>2*60+22.300000000000001</f>
+        <f>2*60+22.3</f>
         <v>142.30000000000001</v>
       </c>
       <c r="C4">
-        <f>$B$2/B4</f>
+        <f t="shared" si="0"/>
         <v>2.6950105411103302</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:16384" ht="13.5">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1313,12 +1730,11 @@
         <v>124.16</v>
       </c>
       <c r="C5">
-        <f>$B$2/B5</f>
+        <f t="shared" si="0"/>
         <v>3.0887564432989691</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:16384" ht="13.5">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1326,12 +1742,11 @@
         <v>110.08</v>
       </c>
       <c r="C6">
-        <f>$B$2/B6</f>
+        <f t="shared" si="0"/>
         <v>3.4838299418604652</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:16384" ht="13.5">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1339,66 +1754,38 @@
         <v>103.05</v>
       </c>
       <c r="C7">
-        <f>$B$2/B7</f>
+        <f t="shared" si="0"/>
         <v>3.7214944201843765</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:16384" ht="13.5">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>96.069999999999993</v>
+        <v>96.07</v>
       </c>
       <c r="C8">
-        <f>$B$2/B8</f>
+        <f t="shared" si="0"/>
         <v>3.9918809201623819</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:16384" ht="13.5">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>92.640000000000001</v>
+        <v>92.64</v>
       </c>
       <c r="C9">
-        <f>$B$2/B9</f>
+        <f t="shared" si="0"/>
         <v>4.139680483592401</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:16384">
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:16384">
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:16384">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:16384">
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:16384">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:16384">
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:16384">
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:16384">
-      <c r="I17" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1407,25 +1794,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:XFD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" style="0" width="9.142307692307693" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>